<commit_message>
cambios usando reglas RAE
</commit_message>
<xml_diff>
--- a/server/data.xlsx
+++ b/server/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="227">
   <si>
     <t>Concepto</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Nombre</t>
   </si>
   <si>
-    <t>Nombre programa</t>
-  </si>
-  <si>
     <t>Número del documento normativo</t>
   </si>
   <si>
@@ -339,9 +336,6 @@
     <t>N799</t>
   </si>
   <si>
-    <t>Nombre proyecto</t>
-  </si>
-  <si>
     <t>N961</t>
   </si>
   <si>
@@ -354,12 +348,6 @@
     <t>F294</t>
   </si>
   <si>
-    <t>noproyecto</t>
-  </si>
-  <si>
-    <t>N821</t>
-  </si>
-  <si>
     <t>padrón</t>
   </si>
   <si>
@@ -441,12 +429,6 @@
     <t>EstTerr</t>
   </si>
   <si>
-    <t>NomProg</t>
-  </si>
-  <si>
-    <t>NomProy</t>
-  </si>
-  <si>
     <t>Ambito aplicación</t>
   </si>
   <si>
@@ -697,12 +679,6 @@
   </si>
   <si>
     <t>Subclase Cobertura Tierra</t>
-  </si>
-  <si>
-    <t>Nombre Proyecto</t>
-  </si>
-  <si>
-    <t>Nombre Programa</t>
   </si>
   <si>
     <t>Número Programa</t>
@@ -1120,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,19 +1117,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1161,19 +1137,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1181,19 +1157,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G3" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1201,19 +1177,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G4" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1221,19 +1197,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>147</v>
-      </c>
       <c r="G5" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1241,16 +1217,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1258,16 +1234,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1275,19 +1251,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1295,22 +1271,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G9" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="H9" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1318,22 +1294,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>71</v>
-      </c>
       <c r="D10" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="G10" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H10" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1341,22 +1317,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="G11" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H11" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1364,22 +1340,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G12" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="H12" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1387,22 +1363,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G13" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H13" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1410,22 +1386,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G14" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="H14" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1433,22 +1409,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G15" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="H15" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1456,22 +1432,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G16" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="H16" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1479,16 +1455,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="D17" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1496,16 +1472,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D18" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1513,16 +1489,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1530,16 +1506,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D20" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1547,16 +1523,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D21" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1564,16 +1540,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1581,16 +1557,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1598,16 +1574,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1615,16 +1591,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D25" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1632,16 +1608,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D26" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1649,10 +1625,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D27" t="s">
         <v>26</v>
@@ -1666,16 +1642,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D28" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1683,10 +1659,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D29" t="s">
         <v>28</v>
@@ -1700,242 +1676,242 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>105</v>
+        <v>98</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="D30" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="C31" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D31" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>99</v>
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D32" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D33" t="s">
-        <v>226</v>
+        <v>32</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>159</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D34" t="s">
-        <v>227</v>
+        <v>33</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D35" t="s">
-        <v>33</v>
+        <v>223</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="D36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="D37" t="s">
+        <v>222</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D37" t="s">
-        <v>231</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C38" s="7" t="s">
+      <c r="D38" t="s">
+        <v>220</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D38" t="s">
-        <v>36</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="D39" t="s">
-        <v>230</v>
+        <v>38</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D40" t="s">
-        <v>228</v>
+        <v>189</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C41" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" t="s">
+        <v>217</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D41" t="s">
-        <v>39</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="5" t="s">
+      <c r="C42" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>128</v>
-      </c>
       <c r="D42" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>129</v>
       </c>
       <c r="D43" t="s">
-        <v>223</v>
+        <v>42</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>130</v>
@@ -1944,44 +1920,10 @@
         <v>131</v>
       </c>
       <c r="D44" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D46" t="s">
-        <v>229</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2005,58 +1947,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>